<commit_message>
home and register page
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Register.xlsx
+++ b/src/test/resources/testdata/Register.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D282D1C3-91E5-48A7-9CAA-A049C0B47154}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaurg\eclipse-workspace\Numpy_DS_Algo\src\test\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31977E4-3089-4EF3-AAA0-3B229DFB488F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +16,6 @@
     <sheet name="registr" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -29,22 +33,31 @@
     <t>password</t>
   </si>
   <si>
-    <t>gagan</t>
-  </si>
-  <si>
-    <t>mahi</t>
-  </si>
-  <si>
     <t>confirm password</t>
   </si>
   <si>
-    <t>abcdefghijk</t>
-  </si>
-  <si>
-    <t>aveersingh</t>
-  </si>
-  <si>
-    <t>abcdefgh</t>
+    <t>message</t>
+  </si>
+  <si>
+    <t>numpy84$3</t>
+  </si>
+  <si>
+    <t>ninja</t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
+    <t>numpy</t>
+  </si>
+  <si>
+    <t>automation</t>
+  </si>
+  <si>
+    <t>automation84</t>
+  </si>
+  <si>
+    <t>ninja5</t>
   </si>
 </sst>
 </file>
@@ -362,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -373,10 +386,10 @@
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="19.1796875" customWidth="1"/>
     <col min="3" max="3" width="28.6328125" customWidth="1"/>
-    <col min="4" max="4" width="17.7265625" customWidth="1"/>
+    <col min="4" max="4" width="52.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -384,28 +397,65 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>123456789</v>
+      </c>
+      <c r="C4">
+        <v>123456789</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>